<commit_message>
se actualizaron los requerimientos del usuario
</commit_message>
<xml_diff>
--- a/Datos del CV. Alexandr.xlsx
+++ b/Datos del CV. Alexandr.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="18975" windowHeight="11145" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="18975" windowHeight="11145"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>CV</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Datos del CV</t>
   </si>
@@ -80,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,114 +116,405 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A6" rightToLeft="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.838095238095235" customWidth="1"/>
+    <col min="1" max="1" width="45.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="60.65" customHeight="1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -234,26 +523,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1" rightToLeft="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1" rightToLeft="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>